<commit_message>
feat: correções algoritmos lucas parte 1
</commit_message>
<xml_diff>
--- a/assets/toy_problem.xlsx
+++ b/assets/toy_problem.xlsx
@@ -192,7 +192,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -222,6 +222,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -477,7 +481,7 @@
   <dimension ref="A1:P1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -542,7 +546,7 @@
       <c r="C2" s="7" t="n">
         <v>1.2</v>
       </c>
-      <c r="D2" s="7" t="n">
+      <c r="D2" s="8" t="n">
         <v>43</v>
       </c>
       <c r="E2" s="7" t="s">
@@ -592,7 +596,7 @@
       <c r="C3" s="7" t="n">
         <v>1.5</v>
       </c>
-      <c r="D3" s="7" t="n">
+      <c r="D3" s="8" t="n">
         <v>35</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -642,7 +646,7 @@
       <c r="C4" s="7" t="n">
         <v>1.2</v>
       </c>
-      <c r="D4" s="7" t="n">
+      <c r="D4" s="8" t="n">
         <v>45</v>
       </c>
       <c r="E4" s="7" t="s">

</xml_diff>